<commit_message>
updated figma diagram for organizer event, adding filled userbacklog
</commit_message>
<xml_diff>
--- a/doc/UserBacklog.xlsx
+++ b/doc/UserBacklog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="155">
   <si>
     <t>ID</t>
   </si>
@@ -39,6 +39,9 @@
     <t>Completed By</t>
   </si>
   <si>
+    <t xml:space="preserve"> = On github</t>
+  </si>
+  <si>
     <t>US 01.01.01</t>
   </si>
   <si>
@@ -430,6 +433,9 @@
   </si>
   <si>
     <t>The software should allow administators to remove images</t>
+  </si>
+  <si>
+    <t>John</t>
   </si>
   <si>
     <t>US 03.04.01</t>
@@ -506,12 +512,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6D9EEB"/>
+        <bgColor rgb="FF6D9EEB"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -534,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -553,8 +571,16 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -804,29 +830,33 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="6">
         <f t="shared" ref="A2:A47" si="1">ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>7</v>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="7">
+      <c r="D2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="8">
         <v>1.0</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>11</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
@@ -835,22 +865,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
@@ -859,22 +889,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="7">
+      <c r="D4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="8">
         <v>1.0</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>11</v>
+      <c r="F4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -883,22 +913,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="7">
+      <c r="D5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="8">
         <v>3.0</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>11</v>
+      <c r="F5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
@@ -907,22 +937,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="7">
+      <c r="D6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="8">
         <v>2.0</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>11</v>
+      <c r="F6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
@@ -931,22 +961,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="7">
+      <c r="D7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="8">
         <v>1.0</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>11</v>
+      <c r="F7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -955,22 +985,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="D8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>11</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
@@ -979,22 +1009,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="7">
+      <c r="D9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="8">
         <v>2.0</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>11</v>
+      <c r="F9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
@@ -1003,857 +1033,1031 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="7">
+      <c r="D10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="8">
         <v>2.0</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25" customHeight="1">
+      <c r="A11" s="9">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="6">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="9" t="s">
         <v>40</v>
       </c>
+      <c r="C11" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="D11" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E11" s="7">
         <v>2.0</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="6">
+      <c r="A12" s="9">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="9" t="s">
         <v>43</v>
       </c>
+      <c r="C12" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="D12" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E12" s="7">
         <v>1.0</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="6">
+      <c r="A13" s="9">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="9" t="s">
         <v>46</v>
       </c>
+      <c r="C13" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="D13" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E13" s="7">
         <v>1.0</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="6">
+      <c r="A14" s="9">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="9" t="s">
         <v>49</v>
       </c>
+      <c r="C14" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="D14" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E14" s="7">
         <v>2.0</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="6">
+      <c r="A15" s="9">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="9" t="s">
         <v>52</v>
       </c>
+      <c r="C15" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="D15" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E15" s="7">
         <v>1.0</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="6">
+      <c r="A16" s="9">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="9" t="s">
         <v>55</v>
       </c>
+      <c r="C16" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="D16" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E16" s="7">
         <v>1.0</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="6">
+      <c r="A17" s="9">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="9" t="s">
         <v>58</v>
       </c>
+      <c r="C17" s="9" t="s">
+        <v>59</v>
+      </c>
       <c r="D17" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E17" s="7">
         <v>1.0</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="6">
+      <c r="A18" s="9">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="9" t="s">
         <v>61</v>
       </c>
+      <c r="C18" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="D18" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E18" s="7">
         <v>3.0</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="6">
+      <c r="A19" s="9">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="9" t="s">
         <v>65</v>
       </c>
+      <c r="C19" s="9" t="s">
+        <v>66</v>
+      </c>
       <c r="D19" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E19" s="7">
         <v>2.0</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="6">
+      <c r="A20" s="9">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="9" t="s">
         <v>68</v>
       </c>
+      <c r="C20" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="D20" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E20" s="7">
         <v>1.0</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="6">
+      <c r="A21" s="9">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="9" t="s">
         <v>71</v>
       </c>
+      <c r="C21" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="D21" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E21" s="7">
         <v>3.0</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="6">
+      <c r="A22" s="9">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="9" t="s">
         <v>74</v>
       </c>
+      <c r="C22" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="D22" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E22" s="7">
         <v>2.0</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="6">
+      <c r="A23" s="9">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="9" t="s">
         <v>77</v>
       </c>
+      <c r="C23" s="9" t="s">
+        <v>78</v>
+      </c>
       <c r="D23" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E23" s="7">
         <v>2.0</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="6">
+      <c r="A24" s="9">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="B24" s="9" t="s">
         <v>80</v>
       </c>
+      <c r="C24" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="D24" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E24" s="7">
         <v>3.0</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="6">
+      <c r="A25" s="9">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="6" t="s">
+      <c r="B25" s="9" t="s">
         <v>83</v>
       </c>
+      <c r="C25" s="9" t="s">
+        <v>84</v>
+      </c>
       <c r="D25" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E25" s="7">
         <v>2.0</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="6">
+      <c r="A26" s="9">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="B26" s="9" t="s">
         <v>86</v>
       </c>
+      <c r="C26" s="9" t="s">
+        <v>87</v>
+      </c>
       <c r="D26" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E26" s="7">
         <v>1.0</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="6">
+      <c r="A27" s="9">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C27" s="6" t="s">
+      <c r="B27" s="9" t="s">
         <v>90</v>
       </c>
+      <c r="C27" s="9" t="s">
+        <v>91</v>
+      </c>
       <c r="D27" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E27" s="7">
         <v>1.0</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="6">
+      <c r="A28" s="9">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="6" t="s">
+      <c r="B28" s="9" t="s">
         <v>93</v>
       </c>
+      <c r="C28" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="D28" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E28" s="7">
         <v>1.0</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="6">
+      <c r="A29" s="9">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29" s="6" t="s">
+      <c r="B29" s="9" t="s">
         <v>96</v>
       </c>
+      <c r="C29" s="9" t="s">
+        <v>97</v>
+      </c>
       <c r="D29" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E29" s="7">
         <v>2.0</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="6">
+      <c r="A30" s="9">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="9" t="s">
         <v>99</v>
       </c>
+      <c r="C30" s="9" t="s">
+        <v>100</v>
+      </c>
       <c r="D30" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E30" s="7">
         <v>1.0</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="6">
+      <c r="A31" s="9">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="B31" s="9" t="s">
         <v>102</v>
       </c>
+      <c r="C31" s="9" t="s">
+        <v>103</v>
+      </c>
       <c r="D31" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E31" s="7">
         <v>2.0</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="6">
+      <c r="A32" s="9">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C32" s="6" t="s">
+      <c r="B32" s="9" t="s">
         <v>105</v>
       </c>
+      <c r="C32" s="9" t="s">
+        <v>106</v>
+      </c>
       <c r="D32" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E32" s="7">
         <v>1.0</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="6">
+      <c r="A33" s="9">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="B33" s="9" t="s">
         <v>108</v>
       </c>
+      <c r="C33" s="9" t="s">
+        <v>109</v>
+      </c>
       <c r="D33" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E33" s="7">
         <v>1.0</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="6">
+      <c r="A34" s="9">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C34" s="6" t="s">
+      <c r="B34" s="9" t="s">
         <v>111</v>
       </c>
+      <c r="C34" s="9" t="s">
+        <v>112</v>
+      </c>
       <c r="D34" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E34" s="7">
         <v>1.0</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="6">
+      <c r="A35" s="9">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C35" s="6" t="s">
+      <c r="B35" s="9" t="s">
         <v>115</v>
       </c>
+      <c r="C35" s="9" t="s">
+        <v>116</v>
+      </c>
       <c r="D35" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E35" s="7">
         <v>2.0</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="6">
+      <c r="A36" s="9">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C36" s="6" t="s">
+      <c r="B36" s="9" t="s">
         <v>118</v>
       </c>
+      <c r="C36" s="9" t="s">
+        <v>119</v>
+      </c>
       <c r="D36" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E36" s="7">
         <v>1.0</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="6">
+      <c r="A37" s="9">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C37" s="6" t="s">
+      <c r="B37" s="9" t="s">
         <v>121</v>
       </c>
+      <c r="C37" s="9" t="s">
+        <v>122</v>
+      </c>
       <c r="D37" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E37" s="7">
         <v>3.0</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="6">
+      <c r="A38" s="9">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C38" s="6" t="s">
+      <c r="B38" s="9" t="s">
         <v>124</v>
       </c>
+      <c r="C38" s="9" t="s">
+        <v>125</v>
+      </c>
       <c r="D38" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E38" s="7">
         <v>3.0</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="6">
+      <c r="A39" s="9">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C39" s="6" t="s">
+      <c r="B39" s="9" t="s">
         <v>127</v>
       </c>
+      <c r="C39" s="9" t="s">
+        <v>128</v>
+      </c>
       <c r="D39" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E39" s="7">
         <v>3.0</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="6">
+      <c r="A40" s="9">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C40" s="6" t="s">
+      <c r="B40" s="9" t="s">
         <v>130</v>
       </c>
+      <c r="C40" s="9" t="s">
+        <v>131</v>
+      </c>
       <c r="D40" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E40" s="7">
         <v>1.0</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="6">
+      <c r="A41" s="9">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C41" s="6" t="s">
+      <c r="B41" s="9" t="s">
         <v>133</v>
       </c>
+      <c r="C41" s="9" t="s">
+        <v>134</v>
+      </c>
       <c r="D41" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E41" s="7">
         <v>1.0</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="6">
+      <c r="A42" s="10">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C42" s="6" t="s">
+      <c r="B42" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="C42" s="10" t="s">
         <v>137</v>
       </c>
+      <c r="D42" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E42" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10"/>
+      <c r="T42" s="10"/>
+      <c r="U42" s="10"/>
+      <c r="V42" s="10"/>
+      <c r="W42" s="10"/>
+      <c r="X42" s="10"/>
+      <c r="Y42" s="10"/>
+      <c r="Z42" s="10"/>
+      <c r="AA42" s="10"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="6">
+      <c r="A43" s="10">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C43" s="6" t="s">
+      <c r="B43" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E43" s="11">
+        <v>2.0</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>140</v>
-      </c>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="10"/>
+      <c r="S43" s="10"/>
+      <c r="T43" s="10"/>
+      <c r="U43" s="10"/>
+      <c r="V43" s="10"/>
+      <c r="W43" s="10"/>
+      <c r="X43" s="10"/>
+      <c r="Y43" s="10"/>
+      <c r="Z43" s="10"/>
+      <c r="AA43" s="10"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="6">
+      <c r="A44" s="10">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="D44" s="7" t="s">
+      <c r="B44" s="10" t="s">
         <v>143</v>
       </c>
+      <c r="C44" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E44" s="11">
+        <v>2.0</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
+      <c r="R44" s="10"/>
+      <c r="S44" s="10"/>
+      <c r="T44" s="10"/>
+      <c r="U44" s="10"/>
+      <c r="V44" s="10"/>
+      <c r="W44" s="10"/>
+      <c r="X44" s="10"/>
+      <c r="Y44" s="10"/>
+      <c r="Z44" s="10"/>
+      <c r="AA44" s="10"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="6">
+      <c r="A45" s="10">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B45" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D45" s="7" t="s">
+      <c r="B45" s="10" t="s">
         <v>146</v>
       </c>
+      <c r="C45" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E45" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
+      <c r="R45" s="10"/>
+      <c r="S45" s="10"/>
+      <c r="T45" s="10"/>
+      <c r="U45" s="10"/>
+      <c r="V45" s="10"/>
+      <c r="W45" s="10"/>
+      <c r="X45" s="10"/>
+      <c r="Y45" s="10"/>
+      <c r="Z45" s="10"/>
+      <c r="AA45" s="10"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="6">
+      <c r="A46" s="10">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B46" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D46" s="7" t="s">
+      <c r="B46" s="10" t="s">
         <v>149</v>
       </c>
+      <c r="C46" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E46" s="11">
+        <v>3.0</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="10"/>
+      <c r="R46" s="10"/>
+      <c r="S46" s="10"/>
+      <c r="T46" s="10"/>
+      <c r="U46" s="10"/>
+      <c r="V46" s="10"/>
+      <c r="W46" s="10"/>
+      <c r="X46" s="10"/>
+      <c r="Y46" s="10"/>
+      <c r="Z46" s="10"/>
+      <c r="AA46" s="10"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="6">
+      <c r="A47" s="10">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="D47" s="7" t="s">
+      <c r="B47" s="10" t="s">
         <v>152</v>
       </c>
+      <c r="C47" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E47" s="11">
+        <v>2.0</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="10"/>
+      <c r="R47" s="10"/>
+      <c r="S47" s="10"/>
+      <c r="T47" s="10"/>
+      <c r="U47" s="10"/>
+      <c r="V47" s="10"/>
+      <c r="W47" s="10"/>
+      <c r="X47" s="10"/>
+      <c r="Y47" s="10"/>
+      <c r="Z47" s="10"/>
+      <c r="AA47" s="10"/>
     </row>
     <row r="48" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>

</xml_diff>